<commit_message>
Updated management files to improve output soil.xlsx.
</commit_message>
<xml_diff>
--- a/data/management/Management_information_DKI_2017.xlsx
+++ b/data/management/Management_information_DKI_2017.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tillrose/Library/Mobile Documents/com~apple~CloudDocs/iCloud Daten/Arbeit/R-Projects/Git_Repositories/BRIWECS_Data_Publication_2/data/management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378A2B2C-E11F-5D43-9875-6F7DE77256D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605D2750-32A3-FE42-BCB2-A4E93484D049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="500" windowWidth="27800" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -268,9 +268,6 @@
     <t>fallow</t>
   </si>
   <si>
-    <t>winterwheat</t>
-  </si>
-  <si>
     <t>Sowing density</t>
   </si>
   <si>
@@ -347,6 +344,9 @@
   </si>
   <si>
     <t>UAN (inhibited)</t>
+  </si>
+  <si>
+    <t>winter wheat</t>
   </si>
 </sst>
 </file>
@@ -861,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E51" sqref="B51:E51"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -928,7 +928,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -950,7 +950,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -993,34 +993,34 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1046,7 +1046,7 @@
         <v>33</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C25" s="1"/>
     </row>
@@ -1055,7 +1055,7 @@
         <v>34</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C26" s="1"/>
     </row>
@@ -1064,7 +1064,7 @@
         <v>35</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C27" s="1"/>
     </row>
@@ -1073,7 +1073,7 @@
         <v>36</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C28" s="1"/>
     </row>
@@ -1082,7 +1082,7 @@
         <v>37</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="C29" s="1"/>
     </row>
@@ -1152,7 +1152,7 @@
         <v>45</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C37" s="1"/>
     </row>
@@ -1161,7 +1161,7 @@
         <v>62</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C38" s="15">
         <v>41518</v>
@@ -1172,7 +1172,7 @@
         <v>63</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C39" s="15">
         <v>41518</v>
@@ -1190,7 +1190,7 @@
         <v>47</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C41" s="15">
         <v>42797</v>
@@ -1201,7 +1201,7 @@
         <v>49</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C42" s="15">
         <v>42797</v>
@@ -1212,7 +1212,7 @@
         <v>50</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C43" s="15">
         <v>42797</v>
@@ -1223,7 +1223,7 @@
         <v>48</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C44" s="15">
         <v>42797</v>
@@ -1234,7 +1234,7 @@
         <v>51</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C45" s="1"/>
     </row>
@@ -1264,7 +1264,7 @@
         <v>6</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E48" s="10" t="s">
         <v>7</v>
@@ -1276,7 +1276,7 @@
         <v>6</v>
       </c>
       <c r="H48" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I48" s="10" t="s">
         <v>7</v>
@@ -1302,7 +1302,7 @@
         <v>50</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>11</v>
@@ -1333,7 +1333,7 @@
         <v>124</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>12</v>

</xml_diff>